<commit_message>
Update: Threat Alert Report - 2026-01-10 08:08
</commit_message>
<xml_diff>
--- a/excel_routes/route_CAI_DMM_threats.xlsx
+++ b/excel_routes/route_CAI_DMM_threats.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -537,7 +537,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>09-JAN-26</t>
+          <t>13-JAN-26</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -547,17 +547,17 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>Nesma Airlines NE-150</t>
+          <t>Nile Air NP-131</t>
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>8140</v>
+        <v>11341</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>9907</v>
+        <v>11858</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>-1767</v>
+        <v>-517</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>30</v>
@@ -582,7 +582,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>09-JAN-26</t>
+          <t>13-JAN-26</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -592,26 +592,26 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>flynas XY-895</t>
+          <t>Nesma Airlines NE-150</t>
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>8190</v>
+        <v>11618</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>9907</v>
+        <v>11858</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>-1717</v>
+        <v>-240</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H3" s="2" t="n">
         <v>30</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J3" s="3" t="inlineStr">
         <is>
@@ -627,7 +627,7 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>10-JAN-26</t>
+          <t>13-JAN-26</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -637,26 +637,26 @@
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>flyadeal F3-912</t>
+          <t>flynas XY-855</t>
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>7307</v>
+        <v>13345</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>9907</v>
+        <v>11858</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>-2600</v>
+        <v>1487</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>30</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>15</v>
+        <v>-10</v>
       </c>
       <c r="J4" s="3" t="inlineStr">
         <is>
@@ -672,7 +672,7 @@
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>10-JAN-26</t>
+          <t>15-JAN-26</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -682,17 +682,17 @@
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>Nile Air NP-131</t>
+          <t>Nesma Airlines NE-154</t>
         </is>
       </c>
       <c r="D5" s="2" t="n">
-        <v>9427</v>
+        <v>11618</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>9907</v>
+        <v>13155</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>-480</v>
+        <v>-1537</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>30</v>
@@ -717,7 +717,7 @@
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>13-JAN-26</t>
+          <t>15-JAN-26</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -727,26 +727,26 @@
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>Nesma Airlines NE-150</t>
+          <t>EgyptAir MS-681</t>
         </is>
       </c>
       <c r="D6" s="2" t="n">
-        <v>8758</v>
+        <v>14693</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>9907</v>
+        <v>13155</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>-1149</v>
+        <v>1538</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="H6" s="2" t="n">
         <v>30</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>0</v>
+        <v>-16</v>
       </c>
       <c r="J6" s="3" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>13-JAN-26</t>
+          <t>16-JAN-26</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -772,17 +772,17 @@
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>Nesma Airlines NE-154</t>
+          <t>Nile Air NP-133</t>
         </is>
       </c>
       <c r="D7" s="2" t="n">
-        <v>9137</v>
+        <v>11341</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>9907</v>
+        <v>14453</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>-770</v>
+        <v>-3112</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>30</v>
@@ -793,9 +793,9 @@
       <c r="I7" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="J7" s="3" t="inlineStr">
-        <is>
-          <t>LOW THREAT</t>
+      <c r="J7" s="4" t="inlineStr">
+        <is>
+          <t>MEDIUM THREAT - MONITOR</t>
         </is>
       </c>
       <c r="K7" s="2" t="inlineStr">
@@ -807,7 +807,7 @@
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>15-JAN-26</t>
+          <t>17-JAN-26</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -817,30 +817,30 @@
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>flynas XY-895</t>
+          <t>Nesma Airlines NE-154</t>
         </is>
       </c>
       <c r="D8" s="2" t="n">
-        <v>10967</v>
+        <v>11618</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>13163</v>
+        <v>14453</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>-2196</v>
+        <v>-2835</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H8" s="2" t="n">
         <v>30</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="J8" s="3" t="inlineStr">
-        <is>
-          <t>LOW THREAT</t>
+        <v>0</v>
+      </c>
+      <c r="J8" s="4" t="inlineStr">
+        <is>
+          <t>MEDIUM THREAT - MONITOR</t>
         </is>
       </c>
       <c r="K8" s="2" t="inlineStr">
@@ -852,7 +852,7 @@
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>15-JAN-26</t>
+          <t>17-JAN-26</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
@@ -862,17 +862,17 @@
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>Nesma Airlines NE-154</t>
+          <t>Nesma Airlines NE-152</t>
         </is>
       </c>
       <c r="D9" s="2" t="n">
-        <v>12936</v>
+        <v>12929</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>13163</v>
+        <v>14453</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>-227</v>
+        <v>-1524</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>30</v>
@@ -897,7 +897,7 @@
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>16-JAN-26</t>
+          <t>22-JAN-26</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -907,17 +907,17 @@
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>Nile Air NP-133</t>
+          <t>Nile Air NP-131</t>
         </is>
       </c>
       <c r="D10" s="2" t="n">
-        <v>11333</v>
+        <v>10207</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>14463</v>
+        <v>10887</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>-3130</v>
+        <v>-680</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>30</v>
@@ -928,9 +928,9 @@
       <c r="I10" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="J10" s="4" t="inlineStr">
-        <is>
-          <t>MEDIUM THREAT - MONITOR</t>
+      <c r="J10" s="3" t="inlineStr">
+        <is>
+          <t>LOW THREAT</t>
         </is>
       </c>
       <c r="K10" s="2" t="inlineStr">
@@ -942,7 +942,7 @@
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>16-JAN-26</t>
+          <t>22-JAN-26</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
@@ -952,30 +952,30 @@
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>Nesma Airlines NE-150</t>
+          <t>EgyptAir MS-681</t>
         </is>
       </c>
       <c r="D11" s="2" t="n">
-        <v>11636</v>
+        <v>12450</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>14463</v>
+        <v>10887</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>-2827</v>
+        <v>1563</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="H11" s="2" t="n">
         <v>30</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" s="4" t="inlineStr">
-        <is>
-          <t>MEDIUM THREAT - MONITOR</t>
+        <v>-16</v>
+      </c>
+      <c r="J11" s="3" t="inlineStr">
+        <is>
+          <t>LOW THREAT</t>
         </is>
       </c>
       <c r="K11" s="2" t="inlineStr">
@@ -987,7 +987,7 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>17-JAN-26</t>
+          <t>24-JAN-26</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -997,17 +997,17 @@
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>Nesma Airlines NE-154</t>
+          <t>Air Arabia Egypt E5-315</t>
         </is>
       </c>
       <c r="D12" s="2" t="n">
-        <v>11636</v>
+        <v>9119</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>13163</v>
+        <v>9904</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>-1527</v>
+        <v>-785</v>
       </c>
       <c r="G12" s="2" t="n">
         <v>30</v>
@@ -1032,7 +1032,7 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>17-JAN-26</t>
+          <t>27-JAN-26</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1042,26 +1042,26 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Nesma Airlines NE-152</t>
+          <t>EgyptAir MS-681</t>
         </is>
       </c>
       <c r="D13" s="2" t="n">
-        <v>11636</v>
+        <v>8316</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>13163</v>
+        <v>6792</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>-1527</v>
+        <v>1524</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="H13" s="2" t="n">
         <v>30</v>
       </c>
       <c r="I13" s="2" t="n">
-        <v>0</v>
+        <v>-16</v>
       </c>
       <c r="J13" s="3" t="inlineStr">
         <is>
@@ -1077,7 +1077,7 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>20-JAN-26</t>
+          <t>30-JAN-26</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1087,26 +1087,26 @@
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>Nesma Airlines NE-154</t>
+          <t>EgyptAir MS-681</t>
         </is>
       </c>
       <c r="D14" s="2" t="n">
-        <v>9137</v>
+        <v>8417</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>9907</v>
+        <v>6792</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>-770</v>
+        <v>1625</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="H14" s="2" t="n">
         <v>30</v>
       </c>
       <c r="I14" s="2" t="n">
-        <v>0</v>
+        <v>-16</v>
       </c>
       <c r="J14" s="3" t="inlineStr">
         <is>
@@ -1122,7 +1122,7 @@
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>20-JAN-26</t>
+          <t>31-JAN-26</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1132,17 +1132,17 @@
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>Nesma Airlines NE-150</t>
+          <t>Air Arabia Egypt E5-315</t>
         </is>
       </c>
       <c r="D15" s="2" t="n">
-        <v>9137</v>
+        <v>6293</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>9907</v>
+        <v>7434</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>-770</v>
+        <v>-1141</v>
       </c>
       <c r="G15" s="2" t="n">
         <v>30</v>
@@ -1167,7 +1167,7 @@
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>23-JAN-26</t>
+          <t>31-JAN-26</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
@@ -1177,17 +1177,17 @@
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>Nesma Airlines NE-152</t>
+          <t>Nesma Airlines NE-154</t>
         </is>
       </c>
       <c r="D16" s="2" t="n">
-        <v>10349</v>
+        <v>6830</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>10891</v>
+        <v>7434</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>-542</v>
+        <v>-604</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>30</v>
@@ -1212,7 +1212,7 @@
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>24-JAN-26</t>
+          <t>31-JAN-26</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -1222,26 +1222,26 @@
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>Air Arabia Egypt E5-315</t>
+          <t>EgyptAir MS-681</t>
         </is>
       </c>
       <c r="D17" s="2" t="n">
-        <v>8662</v>
+        <v>8316</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>8935</v>
+        <v>7434</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>-273</v>
+        <v>882</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="H17" s="2" t="n">
         <v>30</v>
       </c>
       <c r="I17" s="2" t="n">
-        <v>0</v>
+        <v>-16</v>
       </c>
       <c r="J17" s="3" t="inlineStr">
         <is>
@@ -1249,321 +1249,6 @@
         </is>
       </c>
       <c r="K17" s="2" t="inlineStr">
-        <is>
-          <t>EGP</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="inlineStr">
-        <is>
-          <t>24-JAN-26</t>
-        </is>
-      </c>
-      <c r="B18" s="2" t="inlineStr">
-        <is>
-          <t>SM-433</t>
-        </is>
-      </c>
-      <c r="C18" s="2" t="inlineStr">
-        <is>
-          <t>Nesma Airlines NE-154</t>
-        </is>
-      </c>
-      <c r="D18" s="2" t="n">
-        <v>8758</v>
-      </c>
-      <c r="E18" s="2" t="n">
-        <v>8935</v>
-      </c>
-      <c r="F18" s="2" t="n">
-        <v>-177</v>
-      </c>
-      <c r="G18" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="H18" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="I18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" s="3" t="inlineStr">
-        <is>
-          <t>LOW THREAT</t>
-        </is>
-      </c>
-      <c r="K18" s="2" t="inlineStr">
-        <is>
-          <t>EGP</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="inlineStr">
-        <is>
-          <t>29-JAN-26</t>
-        </is>
-      </c>
-      <c r="B19" s="2" t="inlineStr">
-        <is>
-          <t>SM-433</t>
-        </is>
-      </c>
-      <c r="C19" s="2" t="inlineStr">
-        <is>
-          <t>EgyptAir MS-683</t>
-        </is>
-      </c>
-      <c r="D19" s="2" t="n">
-        <v>8127</v>
-      </c>
-      <c r="E19" s="2" t="n">
-        <v>6789</v>
-      </c>
-      <c r="F19" s="2" t="n">
-        <v>1338</v>
-      </c>
-      <c r="G19" s="2" t="n">
-        <v>46</v>
-      </c>
-      <c r="H19" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="I19" s="2" t="n">
-        <v>-16</v>
-      </c>
-      <c r="J19" s="3" t="inlineStr">
-        <is>
-          <t>LOW THREAT</t>
-        </is>
-      </c>
-      <c r="K19" s="2" t="inlineStr">
-        <is>
-          <t>EGP</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="inlineStr">
-        <is>
-          <t>30-JAN-26</t>
-        </is>
-      </c>
-      <c r="B20" s="2" t="inlineStr">
-        <is>
-          <t>SM-433</t>
-        </is>
-      </c>
-      <c r="C20" s="2" t="inlineStr">
-        <is>
-          <t>EgyptAir MS-681</t>
-        </is>
-      </c>
-      <c r="D20" s="2" t="n">
-        <v>8228</v>
-      </c>
-      <c r="E20" s="2" t="n">
-        <v>6209</v>
-      </c>
-      <c r="F20" s="2" t="n">
-        <v>2019</v>
-      </c>
-      <c r="G20" s="2" t="n">
-        <v>46</v>
-      </c>
-      <c r="H20" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="I20" s="2" t="n">
-        <v>-16</v>
-      </c>
-      <c r="J20" s="3" t="inlineStr">
-        <is>
-          <t>LOW THREAT</t>
-        </is>
-      </c>
-      <c r="K20" s="2" t="inlineStr">
-        <is>
-          <t>EGP</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="inlineStr">
-        <is>
-          <t>31-JAN-26</t>
-        </is>
-      </c>
-      <c r="B21" s="2" t="inlineStr">
-        <is>
-          <t>SM-433</t>
-        </is>
-      </c>
-      <c r="C21" s="2" t="inlineStr">
-        <is>
-          <t>flynas XY-855</t>
-        </is>
-      </c>
-      <c r="D21" s="2" t="n">
-        <v>5919</v>
-      </c>
-      <c r="E21" s="2" t="n">
-        <v>7446</v>
-      </c>
-      <c r="F21" s="2" t="n">
-        <v>-1527</v>
-      </c>
-      <c r="G21" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="H21" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="I21" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="J21" s="3" t="inlineStr">
-        <is>
-          <t>LOW THREAT</t>
-        </is>
-      </c>
-      <c r="K21" s="2" t="inlineStr">
-        <is>
-          <t>EGP</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>31-JAN-26</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="inlineStr">
-        <is>
-          <t>SM-433</t>
-        </is>
-      </c>
-      <c r="C22" s="2" t="inlineStr">
-        <is>
-          <t>Air Arabia Egypt E5-315</t>
-        </is>
-      </c>
-      <c r="D22" s="2" t="n">
-        <v>6304</v>
-      </c>
-      <c r="E22" s="2" t="n">
-        <v>7446</v>
-      </c>
-      <c r="F22" s="2" t="n">
-        <v>-1142</v>
-      </c>
-      <c r="G22" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="H22" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="I22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" s="3" t="inlineStr">
-        <is>
-          <t>LOW THREAT</t>
-        </is>
-      </c>
-      <c r="K22" s="2" t="inlineStr">
-        <is>
-          <t>EGP</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="2" t="inlineStr">
-        <is>
-          <t>31-JAN-26</t>
-        </is>
-      </c>
-      <c r="B23" s="2" t="inlineStr">
-        <is>
-          <t>SM-433</t>
-        </is>
-      </c>
-      <c r="C23" s="2" t="inlineStr">
-        <is>
-          <t>Nesma Airlines NE-154</t>
-        </is>
-      </c>
-      <c r="D23" s="2" t="n">
-        <v>6436</v>
-      </c>
-      <c r="E23" s="2" t="n">
-        <v>7446</v>
-      </c>
-      <c r="F23" s="2" t="n">
-        <v>-1010</v>
-      </c>
-      <c r="G23" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="H23" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="I23" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J23" s="3" t="inlineStr">
-        <is>
-          <t>LOW THREAT</t>
-        </is>
-      </c>
-      <c r="K23" s="2" t="inlineStr">
-        <is>
-          <t>EGP</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="2" t="inlineStr">
-        <is>
-          <t>31-JAN-26</t>
-        </is>
-      </c>
-      <c r="B24" s="2" t="inlineStr">
-        <is>
-          <t>SM-433</t>
-        </is>
-      </c>
-      <c r="C24" s="2" t="inlineStr">
-        <is>
-          <t>EgyptAir MS-681</t>
-        </is>
-      </c>
-      <c r="D24" s="2" t="n">
-        <v>9276</v>
-      </c>
-      <c r="E24" s="2" t="n">
-        <v>7446</v>
-      </c>
-      <c r="F24" s="2" t="n">
-        <v>1830</v>
-      </c>
-      <c r="G24" s="2" t="n">
-        <v>46</v>
-      </c>
-      <c r="H24" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="I24" s="2" t="n">
-        <v>-16</v>
-      </c>
-      <c r="J24" s="3" t="inlineStr">
-        <is>
-          <t>LOW THREAT</t>
-        </is>
-      </c>
-      <c r="K24" s="2" t="inlineStr">
         <is>
           <t>EGP</t>
         </is>

</xml_diff>

<commit_message>
Update: Threat Alert Report - 2026-01-10 08:46
</commit_message>
<xml_diff>
--- a/excel_routes/route_CAI_DMM_threats.xlsx
+++ b/excel_routes/route_CAI_DMM_threats.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -627,7 +627,7 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>13-JAN-26</t>
+          <t>15-JAN-26</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -637,26 +637,26 @@
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>flynas XY-855</t>
+          <t>EgyptAir MS-681</t>
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>13345</v>
+        <v>14693</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>11858</v>
+        <v>13155</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>1487</v>
+        <v>1538</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>30</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>-10</v>
+        <v>-16</v>
       </c>
       <c r="J4" s="3" t="inlineStr">
         <is>
@@ -672,7 +672,7 @@
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>15-JAN-26</t>
+          <t>16-JAN-26</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -682,17 +682,17 @@
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>Nesma Airlines NE-154</t>
+          <t>Nile Air NP-133</t>
         </is>
       </c>
       <c r="D5" s="2" t="n">
-        <v>11618</v>
+        <v>11341</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>13155</v>
+        <v>14453</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>-1537</v>
+        <v>-3112</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>30</v>
@@ -703,9 +703,9 @@
       <c r="I5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="J5" s="3" t="inlineStr">
-        <is>
-          <t>LOW THREAT</t>
+      <c r="J5" s="4" t="inlineStr">
+        <is>
+          <t>MEDIUM THREAT - MONITOR</t>
         </is>
       </c>
       <c r="K5" s="2" t="inlineStr">
@@ -717,7 +717,7 @@
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>15-JAN-26</t>
+          <t>17-JAN-26</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -727,30 +727,30 @@
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>EgyptAir MS-681</t>
+          <t>Nesma Airlines NE-154</t>
         </is>
       </c>
       <c r="D6" s="2" t="n">
-        <v>14693</v>
+        <v>11618</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>13155</v>
+        <v>14453</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>1538</v>
+        <v>-2835</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="H6" s="2" t="n">
         <v>30</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>-16</v>
-      </c>
-      <c r="J6" s="3" t="inlineStr">
-        <is>
-          <t>LOW THREAT</t>
+        <v>0</v>
+      </c>
+      <c r="J6" s="4" t="inlineStr">
+        <is>
+          <t>MEDIUM THREAT - MONITOR</t>
         </is>
       </c>
       <c r="K6" s="2" t="inlineStr">
@@ -762,7 +762,7 @@
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>16-JAN-26</t>
+          <t>17-JAN-26</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -772,17 +772,17 @@
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>Nile Air NP-133</t>
+          <t>Nesma Airlines NE-152</t>
         </is>
       </c>
       <c r="D7" s="2" t="n">
-        <v>11341</v>
+        <v>12929</v>
       </c>
       <c r="E7" s="2" t="n">
         <v>14453</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>-3112</v>
+        <v>-1524</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>30</v>
@@ -793,9 +793,9 @@
       <c r="I7" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="J7" s="4" t="inlineStr">
-        <is>
-          <t>MEDIUM THREAT - MONITOR</t>
+      <c r="J7" s="3" t="inlineStr">
+        <is>
+          <t>LOW THREAT</t>
         </is>
       </c>
       <c r="K7" s="2" t="inlineStr">
@@ -807,7 +807,7 @@
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>17-JAN-26</t>
+          <t>22-JAN-26</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -817,17 +817,17 @@
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>Nesma Airlines NE-154</t>
+          <t>Nile Air NP-131</t>
         </is>
       </c>
       <c r="D8" s="2" t="n">
-        <v>11618</v>
+        <v>10207</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>14453</v>
+        <v>10887</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>-2835</v>
+        <v>-680</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>30</v>
@@ -838,9 +838,9 @@
       <c r="I8" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="J8" s="4" t="inlineStr">
-        <is>
-          <t>MEDIUM THREAT - MONITOR</t>
+      <c r="J8" s="3" t="inlineStr">
+        <is>
+          <t>LOW THREAT</t>
         </is>
       </c>
       <c r="K8" s="2" t="inlineStr">
@@ -852,7 +852,7 @@
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>17-JAN-26</t>
+          <t>22-JAN-26</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
@@ -862,26 +862,26 @@
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>Nesma Airlines NE-152</t>
+          <t>EgyptAir MS-681</t>
         </is>
       </c>
       <c r="D9" s="2" t="n">
-        <v>12929</v>
+        <v>12450</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>14453</v>
+        <v>10887</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>-1524</v>
+        <v>1563</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="H9" s="2" t="n">
         <v>30</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>0</v>
+        <v>-16</v>
       </c>
       <c r="J9" s="3" t="inlineStr">
         <is>
@@ -897,7 +897,7 @@
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>22-JAN-26</t>
+          <t>24-JAN-26</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -907,17 +907,17 @@
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>Nile Air NP-131</t>
+          <t>Air Arabia Egypt E5-315</t>
         </is>
       </c>
       <c r="D10" s="2" t="n">
-        <v>10207</v>
+        <v>9119</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>10887</v>
+        <v>9904</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>-680</v>
+        <v>-785</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>30</v>
@@ -942,7 +942,7 @@
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>22-JAN-26</t>
+          <t>27-JAN-26</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
@@ -956,13 +956,13 @@
         </is>
       </c>
       <c r="D11" s="2" t="n">
-        <v>12450</v>
+        <v>8316</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>10887</v>
+        <v>6792</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>1563</v>
+        <v>1524</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>46</v>
@@ -987,7 +987,7 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>24-JAN-26</t>
+          <t>30-JAN-26</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -997,26 +997,26 @@
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>Air Arabia Egypt E5-315</t>
+          <t>EgyptAir MS-681</t>
         </is>
       </c>
       <c r="D12" s="2" t="n">
-        <v>9119</v>
+        <v>8417</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>9904</v>
+        <v>6792</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>-785</v>
+        <v>1625</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="H12" s="2" t="n">
         <v>30</v>
       </c>
       <c r="I12" s="2" t="n">
-        <v>0</v>
+        <v>-16</v>
       </c>
       <c r="J12" s="3" t="inlineStr">
         <is>
@@ -1032,7 +1032,7 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>27-JAN-26</t>
+          <t>31-JAN-26</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1042,26 +1042,26 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>EgyptAir MS-681</t>
+          <t>Air Arabia Egypt E5-315</t>
         </is>
       </c>
       <c r="D13" s="2" t="n">
-        <v>8316</v>
+        <v>6293</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>6792</v>
+        <v>7434</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>1524</v>
+        <v>-1141</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="H13" s="2" t="n">
         <v>30</v>
       </c>
       <c r="I13" s="2" t="n">
-        <v>-16</v>
+        <v>0</v>
       </c>
       <c r="J13" s="3" t="inlineStr">
         <is>
@@ -1077,7 +1077,7 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>30-JAN-26</t>
+          <t>31-JAN-26</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1087,26 +1087,26 @@
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>EgyptAir MS-681</t>
+          <t>Nesma Airlines NE-154</t>
         </is>
       </c>
       <c r="D14" s="2" t="n">
-        <v>8417</v>
+        <v>6830</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>6792</v>
+        <v>7434</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>1625</v>
+        <v>-604</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="H14" s="2" t="n">
         <v>30</v>
       </c>
       <c r="I14" s="2" t="n">
-        <v>-16</v>
+        <v>0</v>
       </c>
       <c r="J14" s="3" t="inlineStr">
         <is>
@@ -1132,26 +1132,26 @@
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>Air Arabia Egypt E5-315</t>
+          <t>EgyptAir MS-681</t>
         </is>
       </c>
       <c r="D15" s="2" t="n">
-        <v>6293</v>
+        <v>8316</v>
       </c>
       <c r="E15" s="2" t="n">
         <v>7434</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>-1141</v>
+        <v>882</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="H15" s="2" t="n">
         <v>30</v>
       </c>
       <c r="I15" s="2" t="n">
-        <v>0</v>
+        <v>-16</v>
       </c>
       <c r="J15" s="3" t="inlineStr">
         <is>
@@ -1159,96 +1159,6 @@
         </is>
       </c>
       <c r="K15" s="2" t="inlineStr">
-        <is>
-          <t>EGP</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="inlineStr">
-        <is>
-          <t>31-JAN-26</t>
-        </is>
-      </c>
-      <c r="B16" s="2" t="inlineStr">
-        <is>
-          <t>SM-433</t>
-        </is>
-      </c>
-      <c r="C16" s="2" t="inlineStr">
-        <is>
-          <t>Nesma Airlines NE-154</t>
-        </is>
-      </c>
-      <c r="D16" s="2" t="n">
-        <v>6830</v>
-      </c>
-      <c r="E16" s="2" t="n">
-        <v>7434</v>
-      </c>
-      <c r="F16" s="2" t="n">
-        <v>-604</v>
-      </c>
-      <c r="G16" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="H16" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="I16" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" s="3" t="inlineStr">
-        <is>
-          <t>LOW THREAT</t>
-        </is>
-      </c>
-      <c r="K16" s="2" t="inlineStr">
-        <is>
-          <t>EGP</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="inlineStr">
-        <is>
-          <t>31-JAN-26</t>
-        </is>
-      </c>
-      <c r="B17" s="2" t="inlineStr">
-        <is>
-          <t>SM-433</t>
-        </is>
-      </c>
-      <c r="C17" s="2" t="inlineStr">
-        <is>
-          <t>EgyptAir MS-681</t>
-        </is>
-      </c>
-      <c r="D17" s="2" t="n">
-        <v>8316</v>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>7434</v>
-      </c>
-      <c r="F17" s="2" t="n">
-        <v>882</v>
-      </c>
-      <c r="G17" s="2" t="n">
-        <v>46</v>
-      </c>
-      <c r="H17" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="I17" s="2" t="n">
-        <v>-16</v>
-      </c>
-      <c r="J17" s="3" t="inlineStr">
-        <is>
-          <t>LOW THREAT</t>
-        </is>
-      </c>
-      <c r="K17" s="2" t="inlineStr">
         <is>
           <t>EGP</t>
         </is>

</xml_diff>